<commit_message>
First exercise of list 3 solved (withou logical normalization)
</commit_message>
<xml_diff>
--- a/Segundo Semestre/Aula_08-11/Normalizacao_exercicio_um.xlsx
+++ b/Segundo Semestre/Aula_08-11/Normalizacao_exercicio_um.xlsx
@@ -8,17 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa\Documents\IFPR\Banco de Dados\Segundo Semestre\Aula_08-11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD21398-37E2-4A9B-AF83-8F2C4962B7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DFA7A4-E4C7-4D24-9625-8B221B310FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{A9708B30-DE49-48DC-9C76-C48CFB201432}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="9" xr2:uid="{A9708B30-DE49-48DC-9C76-C48CFB201432}"/>
   </bookViews>
   <sheets>
     <sheet name="Pessoa" sheetId="1" r:id="rId1"/>
     <sheet name="Sócio" sheetId="2" r:id="rId2"/>
     <sheet name="Funcionário" sheetId="3" r:id="rId3"/>
     <sheet name="Aluno" sheetId="4" r:id="rId4"/>
+    <sheet name="Piloto" sheetId="6" r:id="rId5"/>
+    <sheet name="Instrutor" sheetId="9" r:id="rId6"/>
+    <sheet name="Saída" sheetId="7" r:id="rId7"/>
+    <sheet name="Instrutor_Curso" sheetId="10" r:id="rId8"/>
+    <sheet name="Curso" sheetId="11" r:id="rId9"/>
+    <sheet name="Instituição" sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +35,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="117">
   <si>
     <t>Nome da Entidade</t>
   </si>
@@ -75,9 +80,6 @@
     <t>Descrição  estendida e observações</t>
   </si>
   <si>
-    <t>Id</t>
-  </si>
-  <si>
     <t>Identificador</t>
   </si>
   <si>
@@ -135,9 +137,6 @@
     <t>Matrícula</t>
   </si>
   <si>
-    <t>Representa o código do sócio. Não nulo.</t>
-  </si>
-  <si>
     <t>Numero_horas_voo</t>
   </si>
   <si>
@@ -195,16 +194,205 @@
     <t>Elementos de Dados:</t>
   </si>
   <si>
-    <t>1:M</t>
-  </si>
-  <si>
     <t xml:space="preserve">Representa o código da pessoa, com o qual a saída se relaciona. </t>
   </si>
   <si>
-    <t>Saída_FK_Id_Pessoa_Aluno</t>
-  </si>
-  <si>
     <t>N:1</t>
+  </si>
+  <si>
+    <t>Aluno_FK_Instrutor_Piloto_Numero_breve</t>
+  </si>
+  <si>
+    <t>Representa o número de brevê do piloto, que também é um instrutor.</t>
+  </si>
+  <si>
+    <t>N:N</t>
+  </si>
+  <si>
+    <t>Aluno_FK_Id_Instrutor_Piloto_numero_breve</t>
+  </si>
+  <si>
+    <t>CP e CE</t>
+  </si>
+  <si>
+    <t>Representa o código herdado de pessoa. Não nulo.</t>
+  </si>
+  <si>
+    <t>Status_elegibilidade_voo</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>Representa a condição de se o aluno está apto para virar piloto. Não nulo.</t>
+  </si>
+  <si>
+    <t>Piloto</t>
+  </si>
+  <si>
+    <t>Pil</t>
+  </si>
+  <si>
+    <t>Entidade que define os atributos de um piloto do sistema.</t>
+  </si>
+  <si>
+    <t>Numero_breve</t>
+  </si>
+  <si>
+    <t>Representa o código que descreve unicamente cada piloto. Não nulo.</t>
+  </si>
+  <si>
+    <t>Sai</t>
+  </si>
+  <si>
+    <t>Entidade que define o relacionamento de saída entre alunos e instrutores.</t>
+  </si>
+  <si>
+    <t>1:N</t>
+  </si>
+  <si>
+    <t>Instrutor_FK_Id_Instrutor_Piloto_numero_breve</t>
+  </si>
+  <si>
+    <t>Aluno_FK_Socio_Pessoa_matricula</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>Representa a data em que ocorreu o voo. Não nulo.</t>
+  </si>
+  <si>
+    <t>Hora_saida</t>
+  </si>
+  <si>
+    <t>Representa a hora em que se iniciou o voo. Não nulo.</t>
+  </si>
+  <si>
+    <t>Hora_chegada</t>
+  </si>
+  <si>
+    <t>Representa a hora em que se terminou o voo. Não nulo.</t>
+  </si>
+  <si>
+    <t>Ins</t>
+  </si>
+  <si>
+    <t>Entidade que define os atributos de um instrutor do sistema.</t>
+  </si>
+  <si>
+    <t>Curso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Representa o código da pessoa como instrutor, o qual o aluno se relaciona. </t>
+  </si>
+  <si>
+    <t>Matricula</t>
+  </si>
+  <si>
+    <t>Simpes</t>
+  </si>
+  <si>
+    <t>CP E CE</t>
+  </si>
+  <si>
+    <t>Representa o código que descreve uma pessoa. Não nulo.</t>
+  </si>
+  <si>
+    <t>M:1</t>
+  </si>
+  <si>
+    <t>Representa o aluno no relacionamento.</t>
+  </si>
+  <si>
+    <t>Representa o piloto no relacionamento.</t>
+  </si>
+  <si>
+    <t>Instrutor_Curso</t>
+  </si>
+  <si>
+    <t>Ins_Cur</t>
+  </si>
+  <si>
+    <t>Entidade fruto do relacionamento entre n instâncias de instrutor e curso.</t>
+  </si>
+  <si>
+    <t>Id_curso</t>
+  </si>
+  <si>
+    <t>Representa o curso no relacionamento.</t>
+  </si>
+  <si>
+    <t>Aluno_matricula</t>
+  </si>
+  <si>
+    <t>Representa o código do aluno na saída. Não nulo.</t>
+  </si>
+  <si>
+    <t>Instrutor_numero_breve</t>
+  </si>
+  <si>
+    <t>Representa o código do instrutor na saída. Nulo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Representa o código do instrutor no relacionamento. Não nulo. </t>
+  </si>
+  <si>
+    <t>Curso_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Representa o código do curso no relacionamento. Não nulo. </t>
+  </si>
+  <si>
+    <t>Data_fim</t>
+  </si>
+  <si>
+    <t>Data_inicio</t>
+  </si>
+  <si>
+    <t>Diploma</t>
+  </si>
+  <si>
+    <t>Cur</t>
+  </si>
+  <si>
+    <t>Entidade que representa o curso no qual um instrutor é formado.</t>
+  </si>
+  <si>
+    <t>Instituição</t>
+  </si>
+  <si>
+    <t>Instituicao_Id</t>
+  </si>
+  <si>
+    <t>Representa o código da instituição que oferece o determinado curso.</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>Representa unicamente o id do curso oferecido pela instituição. Não nulo.</t>
+  </si>
+  <si>
+    <t>Representa o código que descreve a instituição que oferece o curso. Não nulo.</t>
+  </si>
+  <si>
+    <t>Insti</t>
+  </si>
+  <si>
+    <t>Entidade que define o local que oferta os cursos ministrados aos instrutores.</t>
+  </si>
+  <si>
+    <t>Representa o nome da instituição. Não nulo.</t>
+  </si>
+  <si>
+    <t>Representa o código único da instituição. Não nulo.</t>
   </si>
 </sst>
 </file>
@@ -559,7 +747,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,70 +802,194 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>15</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>19</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>20</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
         <v>23</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
       </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFABCAC0-493D-475D-8E06-BABE75D686F7}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
         <v>19</v>
       </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
       <c r="G11" t="s">
-        <v>27</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -690,7 +1002,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,10 +1017,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -718,7 +1030,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -745,36 +1057,36 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
         <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -784,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E4B1C28-A0F1-4712-8C1C-FB8CC702B0B5}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,10 +1114,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -815,7 +1127,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -842,19 +1154,36 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -864,9 +1193,233 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FCA4C7-82D2-4BD9-9A0A-BE210A24D456}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28763742-A842-4624-A2EA-EFF0049C047F}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B7A124-8BD0-4A1F-A428-B7B8F28FD5B8}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -882,10 +1435,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -895,87 +1448,660 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
         <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DAB6B68-1735-443D-8F5E-74809BCE5CDF}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{227DFDF5-C9E4-48D3-8F0F-4B79DB3EE6E2}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
         <v>18</v>
       </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF26E12F-FDC8-4C07-B8FF-CEC4C2D4352A}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
       <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
         <v>14</v>
       </c>
-      <c r="F12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" t="s">
-        <v>37</v>
+      <c r="G15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>